<commit_message>
chagned to aus dip
</commit_message>
<xml_diff>
--- a/b2/diploma-applications.xlsx
+++ b/b2/diploma-applications.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1034,9 +1034,50 @@
         <v>69031c7063de7ef743a0e666</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>fatima3</v>
+      </c>
+      <c r="B17" t="str">
+        <v>06@gmail.com</v>
+      </c>
+      <c r="C17" t="str">
+        <v>9234556789</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Intermediate</v>
+      </c>
+      <c r="E17" t="str">
+        <v>2024</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Australia</v>
+      </c>
+      <c r="G17" t="str">
+        <v>diploma</v>
+      </c>
+      <c r="H17" t="str">
+        <v>nj</v>
+      </c>
+      <c r="I17" t="str">
+        <v>No</v>
+      </c>
+      <c r="J17" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="K17" t="str">
+        <v>http://localhost:5173/services/applyfordiplomacourses</v>
+      </c>
+      <c r="L17" t="str">
+        <v>30/10/2025, 2:39:14 pm</v>
+      </c>
+      <c r="M17" t="str">
+        <v>69032b3a322bf809ad24b953</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>